<commit_message>
multiple updates to themese and pa's
</commit_message>
<xml_diff>
--- a/app/assets/data/gov_comm_content_db_v2.xlsx
+++ b/app/assets/data/gov_comm_content_db_v2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ruper\govcom_demo\app\assets\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF217CFE-1B7C-4611-A97C-7F291B5A3406}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42F1E7A7-DA1C-41C5-81A5-45FA976EE338}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="825" yWindow="3345" windowWidth="27270" windowHeight="8430" xr2:uid="{8E909C32-E840-4249-98BE-49D60BEC6040}"/>
+    <workbookView xWindow="1110" yWindow="1320" windowWidth="27270" windowHeight="13905" xr2:uid="{8E909C32-E840-4249-98BE-49D60BEC6040}"/>
   </bookViews>
   <sheets>
     <sheet name="overview" sheetId="2" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="88">
   <si>
     <t>pa_id</t>
   </si>
@@ -279,6 +279,36 @@
   </si>
   <si>
     <t>BEST</t>
+  </si>
+  <si>
+    <t>Contract mobilisation and transition</t>
+  </si>
+  <si>
+    <t>Managing delivery and performance</t>
+  </si>
+  <si>
+    <t>Managing contract risk</t>
+  </si>
+  <si>
+    <t>Supply chain, inventory management/stock control (NHS Only)</t>
+  </si>
+  <si>
+    <t>Supply chain, logistics (NHS Only)</t>
+  </si>
+  <si>
+    <t>Applying effective contract terms</t>
+  </si>
+  <si>
+    <t>Procurement/commercial activity, bid evaluation and supplier selection</t>
+  </si>
+  <si>
+    <t>Appropriate risk allocation between parties</t>
+  </si>
+  <si>
+    <t>pa_complete</t>
+  </si>
+  <si>
+    <t>percent_complete</t>
   </si>
 </sst>
 </file>
@@ -320,7 +350,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -331,6 +361,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -649,7 +682,7 @@
   <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:I1"/>
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -822,10 +855,10 @@
         <v>56</v>
       </c>
       <c r="E6" s="1">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>76</v>
@@ -1010,38 +1043,212 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B272B2A3-EC55-4C5B-BF2E-94EF83BB1318}">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="13.42578125" customWidth="1"/>
-    <col min="3" max="4" width="83" customWidth="1"/>
-    <col min="5" max="5" width="19" customWidth="1"/>
-    <col min="6" max="6" width="13.7109375" customWidth="1"/>
+    <col min="1" max="2" width="14.42578125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="83" style="1" customWidth="1"/>
+    <col min="4" max="4" width="51.5703125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="19" style="1" customWidth="1"/>
+    <col min="6" max="6" width="13.7109375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="20.7109375" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="F1" t="s">
-        <v>16</v>
+      <c r="F1" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="B2" s="1">
+        <v>4</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="E2" s="1">
+        <v>10</v>
+      </c>
+      <c r="F2" s="1">
+        <v>5</v>
+      </c>
+      <c r="G2" s="5">
+        <f>(F2/E2)*100</f>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>4.2</v>
+      </c>
+      <c r="B3" s="1">
+        <v>4</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="E3" s="1">
+        <v>10</v>
+      </c>
+      <c r="F3" s="1">
+        <v>10</v>
+      </c>
+      <c r="G3" s="5">
+        <f t="shared" ref="G3:G9" si="0">(F3/E3)*100</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>4.3</v>
+      </c>
+      <c r="B4" s="1">
+        <v>4</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="E4" s="1">
+        <v>6</v>
+      </c>
+      <c r="F4" s="1">
+        <v>0</v>
+      </c>
+      <c r="G4" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="B5" s="1">
+        <v>5</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E5" s="1">
+        <v>11</v>
+      </c>
+      <c r="F5" s="1">
+        <v>0</v>
+      </c>
+      <c r="G5" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>5.2</v>
+      </c>
+      <c r="B6" s="1">
+        <v>5</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="E6" s="1">
+        <v>14</v>
+      </c>
+      <c r="F6" s="1">
+        <v>0</v>
+      </c>
+      <c r="G6" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>5.3</v>
+      </c>
+      <c r="B7" s="1">
+        <v>5</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="E7" s="1">
+        <v>13</v>
+      </c>
+      <c r="F7" s="1">
+        <v>0</v>
+      </c>
+      <c r="G7" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>5.4</v>
+      </c>
+      <c r="B8" s="1">
+        <v>5</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="E8" s="1">
+        <v>12</v>
+      </c>
+      <c r="F8" s="1">
+        <v>0</v>
+      </c>
+      <c r="G8" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>5.5</v>
+      </c>
+      <c r="B9" s="1">
+        <v>5</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E9" s="1">
+        <v>6</v>
+      </c>
+      <c r="F9" s="1">
+        <v>0</v>
+      </c>
+      <c r="G9" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>